<commit_message>
Updated RegisterPage and added Login module
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -8,33 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Projects\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E1EA6C-A7AE-4D55-B73D-72DE2039C11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02DE184-37A0-4AF1-8342-CAF785841F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE1B7439-35CA-4995-8C66-7A3B2EF8E47C}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{CE1B7439-35CA-4995-8C66-7A3B2EF8E47C}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>FristName</t>
   </si>
@@ -61,13 +53,67 @@
   </si>
   <si>
     <t>Aj1234</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Scenario Type</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Login successful</t>
+  </si>
+  <si>
+    <t>invalid_user@mail.com</t>
+  </si>
+  <si>
+    <t>WrongPass</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>Error: Login was unsuccessful</t>
+  </si>
+  <si>
+    <t>Blank username</t>
+  </si>
+  <si>
+    <t>Error: Please enter email</t>
+  </si>
+  <si>
+    <t>Blank password</t>
+  </si>
+  <si>
+    <t>Error: Please enter password</t>
+  </si>
+  <si>
+    <t>Invalid email format</t>
+  </si>
+  <si>
+    <t>Error: Wrong email format</t>
+  </si>
+  <si>
+    <t>Both fields blank</t>
+  </si>
+  <si>
+    <t>Error: Please enter credentials</t>
+  </si>
+  <si>
+    <t>email1@gamil.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +125,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,9 +159,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -425,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC62462-DC93-4936-8AFC-C0DDBFEC3078}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -433,6 +496,7 @@
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -475,4 +539,119 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161AB4B0-3510-481C-8DE6-62D3F728A733}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B049D842-3E88-49A1-93E3-DAC81BD6AF52}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{40392A63-5FCD-4323-87E7-14B425F4E0BE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pushed working AddToCart module, logs, updated readme, and cleanup
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Projects\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02DE184-37A0-4AF1-8342-CAF785841F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3766F5C6-EA40-4D05-9476-175FD7EC43DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{CE1B7439-35CA-4995-8C66-7A3B2EF8E47C}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>FristName</t>
   </si>
@@ -64,49 +64,49 @@
     <t>Expected Result</t>
   </si>
   <si>
-    <t>Valid</t>
-  </si>
-  <si>
     <t>Login successful</t>
   </si>
   <si>
-    <t>invalid_user@mail.com</t>
-  </si>
-  <si>
-    <t>WrongPass</t>
-  </si>
-  <si>
-    <t>Invalid credentials</t>
-  </si>
-  <si>
-    <t>Error: Login was unsuccessful</t>
-  </si>
-  <si>
     <t>Blank username</t>
   </si>
   <si>
-    <t>Error: Please enter email</t>
-  </si>
-  <si>
     <t>Blank password</t>
   </si>
   <si>
-    <t>Error: Please enter password</t>
-  </si>
-  <si>
     <t>Invalid email format</t>
   </si>
   <si>
-    <t>Error: Wrong email format</t>
-  </si>
-  <si>
-    <t>Both fields blank</t>
-  </si>
-  <si>
-    <t>Error: Please enter credentials</t>
-  </si>
-  <si>
-    <t>email1@gamil.com</t>
+    <t>login was unsuccessful</t>
+  </si>
+  <si>
+    <t>no customer account</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address.</t>
+  </si>
+  <si>
+    <t>Ajay.com</t>
+  </si>
+  <si>
+    <t>Sammed@Gmail.com</t>
+  </si>
+  <si>
+    <t>//li[normalize-space()='No customer account found']</t>
+  </si>
+  <si>
+    <t>//span[@for='Email'</t>
+  </si>
+  <si>
+    <t>No customer account found</t>
+  </si>
+  <si>
+    <t>Aj0007@gmail.com</t>
+  </si>
+  <si>
+    <t>Registered User</t>
+  </si>
+  <si>
+    <t>UnRegistered User</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161AB4B0-3510-481C-8DE6-62D3F728A733}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,10 +554,11 @@
     <col min="1" max="1" width="21.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -571,86 +572,85 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3">
-        <v>123456</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3">
-        <v>123456</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3">
-        <v>123456</v>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B049D842-3E88-49A1-93E3-DAC81BD6AF52}"/>
     <hyperlink ref="A5" r:id="rId2" xr:uid="{40392A63-5FCD-4323-87E7-14B425F4E0BE}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{A729E241-E538-4B82-BEA9-66D2AD28FB6A}"/>
+    <hyperlink ref="A6" r:id="rId4" display="email@123.com" xr:uid="{7488AF09-C29A-48AA-9156-C8F79867F5F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>